<commit_message>
Update Release 5 planning
</commit_message>
<xml_diff>
--- a/PMP/Release Planning/Release#5_planning.xlsx
+++ b/PMP/Release Planning/Release#5_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Engineer\OneDrive - MUST University\Desktop\Release#5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C05747-35EC-4B4A-B9E8-AC85B80CA2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1FDBDD-2414-473B-9904-4EAE761DC007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{09E57C9E-5FED-45FA-83CB-16D2930F95A3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
   <si>
     <t>Release Planning</t>
   </si>
@@ -270,6 +270,12 @@
   </si>
   <si>
     <t>Release #5 Planning</t>
+  </si>
+  <si>
+    <t>SCRUM-119</t>
+  </si>
+  <si>
+    <t>Edit SSD Advertisement</t>
   </si>
 </sst>
 </file>
@@ -548,8 +554,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -577,38 +592,65 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -640,95 +682,65 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1066,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{756EBB98-C920-47B4-A4C0-6F8760196D70}">
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:O1"/>
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1083,767 +1095,707 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="H1" s="23" t="s">
+      <c r="D1" s="40"/>
+      <c r="H1" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="25"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="37"/>
     </row>
     <row r="2" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="30" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="H2" s="26" t="s">
+      <c r="D2" s="42"/>
+      <c r="H2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26" t="s">
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
     </row>
     <row r="3" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="30" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="H3" s="27">
+      <c r="D3" s="42"/>
+      <c r="H3" s="39">
         <v>45935</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="27" t="s">
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
     </row>
     <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="30" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="H4" s="26" t="s">
+      <c r="D4" s="42"/>
+      <c r="H4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
     </row>
     <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="30" t="s">
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="H5" s="28" t="s">
+      <c r="D5" s="42"/>
+      <c r="H5" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
     </row>
     <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="30" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
+      <c r="D6" s="42"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
     </row>
     <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="30" t="s">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="H7" s="28" t="s">
+      <c r="D7" s="42"/>
+      <c r="H7" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28" t="s">
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
     </row>
     <row r="12" spans="1:18" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31" t="s">
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31" t="s">
+      <c r="H12" s="21"/>
+      <c r="I12" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31" t="s">
+      <c r="J12" s="21"/>
+      <c r="K12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="31"/>
-      <c r="M12" s="32" t="s">
+      <c r="L12" s="21"/>
+      <c r="M12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="N12" s="32"/>
-      <c r="O12" s="31" t="s">
+      <c r="N12" s="22"/>
+      <c r="O12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31" t="s">
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="R12" s="31"/>
+      <c r="R12" s="21"/>
     </row>
     <row r="13" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="34" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="12" t="s">
+      <c r="E13" s="25"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="12" t="s">
+      <c r="H13" s="14"/>
+      <c r="I13" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="12" t="s">
+      <c r="J13" s="14"/>
+      <c r="K13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="13"/>
-      <c r="M13" s="12">
+      <c r="L13" s="14"/>
+      <c r="M13" s="13">
         <v>2</v>
       </c>
-      <c r="N13" s="13"/>
-      <c r="O13" s="33" t="s">
+      <c r="N13" s="14"/>
+      <c r="O13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="12">
+      <c r="P13" s="14"/>
+      <c r="Q13" s="13">
         <v>1</v>
       </c>
-      <c r="R13" s="13"/>
+      <c r="R13" s="14"/>
     </row>
     <row r="14" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="12" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="10" t="s">
+      <c r="H14" s="14"/>
+      <c r="I14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="10" t="s">
+      <c r="J14" s="2"/>
+      <c r="K14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L14" s="11"/>
-      <c r="M14" s="20">
+      <c r="L14" s="2"/>
+      <c r="M14" s="19">
         <v>4</v>
       </c>
-      <c r="N14" s="11"/>
-      <c r="O14" s="20" t="s">
+      <c r="N14" s="2"/>
+      <c r="O14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="10">
+      <c r="P14" s="2"/>
+      <c r="Q14" s="1">
         <v>1</v>
       </c>
-      <c r="R14" s="11"/>
+      <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="12" t="s">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="10" t="s">
+      <c r="H15" s="14"/>
+      <c r="I15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J15" s="11"/>
-      <c r="K15" s="10" t="s">
+      <c r="J15" s="2"/>
+      <c r="K15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L15" s="11"/>
-      <c r="M15" s="20">
+      <c r="L15" s="2"/>
+      <c r="M15" s="19">
         <v>4</v>
       </c>
-      <c r="N15" s="11"/>
-      <c r="O15" s="20" t="s">
+      <c r="N15" s="2"/>
+      <c r="O15" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="10">
+      <c r="P15" s="2"/>
+      <c r="Q15" s="1">
         <v>1</v>
       </c>
-      <c r="R15" s="11"/>
+      <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:18" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="12" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="18" t="s">
+      <c r="H16" s="14"/>
+      <c r="I16" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="10" t="s">
+      <c r="J16" s="2"/>
+      <c r="K16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="20">
+      <c r="L16" s="2"/>
+      <c r="M16" s="19">
         <v>2</v>
       </c>
-      <c r="N16" s="11"/>
-      <c r="O16" s="20" t="s">
+      <c r="N16" s="2"/>
+      <c r="O16" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="10">
+      <c r="P16" s="2"/>
+      <c r="Q16" s="1">
         <v>1</v>
       </c>
-      <c r="R16" s="11"/>
+      <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="12" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="10" t="s">
+      <c r="H17" s="14"/>
+      <c r="I17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="11"/>
-      <c r="K17" s="10" t="s">
+      <c r="J17" s="2"/>
+      <c r="K17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="11"/>
-      <c r="M17" s="20">
+      <c r="L17" s="2"/>
+      <c r="M17" s="19">
         <v>2</v>
       </c>
-      <c r="N17" s="11"/>
-      <c r="O17" s="20" t="s">
+      <c r="N17" s="2"/>
+      <c r="O17" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="10">
+      <c r="P17" s="2"/>
+      <c r="Q17" s="1">
         <v>1</v>
       </c>
-      <c r="R17" s="11"/>
+      <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="12" t="s">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="18" t="s">
+      <c r="H18" s="14"/>
+      <c r="I18" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="10" t="s">
+      <c r="J18" s="2"/>
+      <c r="K18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L18" s="11"/>
-      <c r="M18" s="20">
+      <c r="L18" s="2"/>
+      <c r="M18" s="19">
         <v>2</v>
       </c>
-      <c r="N18" s="11"/>
-      <c r="O18" s="20" t="s">
+      <c r="N18" s="2"/>
+      <c r="O18" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="10">
+      <c r="P18" s="2"/>
+      <c r="Q18" s="1">
         <v>1</v>
       </c>
-      <c r="R18" s="11"/>
+      <c r="R18" s="2"/>
     </row>
     <row r="19" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="7" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="12" t="s">
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="12" t="s">
+      <c r="H19" s="14"/>
+      <c r="I19" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="12" t="s">
+      <c r="J19" s="14"/>
+      <c r="K19" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="13"/>
-      <c r="M19" s="12">
+      <c r="L19" s="14"/>
+      <c r="M19" s="13">
         <v>2</v>
       </c>
-      <c r="N19" s="13"/>
-      <c r="O19" s="12" t="s">
+      <c r="N19" s="14"/>
+      <c r="O19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="12">
+      <c r="P19" s="14"/>
+      <c r="Q19" s="13">
         <v>1</v>
       </c>
-      <c r="R19" s="13"/>
+      <c r="R19" s="14"/>
     </row>
     <row r="20" spans="1:18" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="12" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="18" t="s">
+      <c r="H20" s="14"/>
+      <c r="I20" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="11"/>
-      <c r="K20" s="10" t="s">
+      <c r="J20" s="2"/>
+      <c r="K20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="11"/>
-      <c r="M20" s="20">
+      <c r="L20" s="2"/>
+      <c r="M20" s="19">
         <v>2</v>
       </c>
-      <c r="N20" s="11"/>
-      <c r="O20" s="20" t="s">
+      <c r="N20" s="2"/>
+      <c r="O20" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="10">
+      <c r="P20" s="2"/>
+      <c r="Q20" s="1">
         <v>1</v>
       </c>
-      <c r="R20" s="11"/>
+      <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="12" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="16" t="s">
+      <c r="H21" s="14"/>
+      <c r="I21" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="J21" s="17"/>
-      <c r="K21" s="16" t="s">
+      <c r="J21" s="16"/>
+      <c r="K21" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="17"/>
-      <c r="M21" s="43">
+      <c r="L21" s="16"/>
+      <c r="M21" s="18">
         <v>2</v>
       </c>
-      <c r="N21" s="17"/>
-      <c r="O21" s="43" t="s">
+      <c r="N21" s="16"/>
+      <c r="O21" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="16">
+      <c r="P21" s="16"/>
+      <c r="Q21" s="17">
         <v>1</v>
       </c>
-      <c r="R21" s="17"/>
+      <c r="R21" s="16"/>
     </row>
     <row r="22" spans="1:18" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="7" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="12" t="s">
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="10" t="s">
+      <c r="H22" s="14"/>
+      <c r="I22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J22" s="11"/>
-      <c r="K22" s="10" t="s">
+      <c r="J22" s="2"/>
+      <c r="K22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="11"/>
-      <c r="M22" s="10">
+      <c r="L22" s="2"/>
+      <c r="M22" s="1">
         <v>2</v>
       </c>
-      <c r="N22" s="11"/>
-      <c r="O22" s="10" t="s">
+      <c r="N22" s="2"/>
+      <c r="O22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="11"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="12" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="18" t="s">
+      <c r="H23" s="14"/>
+      <c r="I23" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="11"/>
-      <c r="K23" s="10" t="s">
+      <c r="J23" s="2"/>
+      <c r="K23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L23" s="11"/>
-      <c r="M23" s="10">
+      <c r="L23" s="2"/>
+      <c r="M23" s="1">
         <v>2</v>
       </c>
-      <c r="N23" s="11"/>
-      <c r="O23" s="10" t="s">
+      <c r="N23" s="2"/>
+      <c r="O23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="11"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="14" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="H24" s="15"/>
-      <c r="I24" s="19" t="s">
+      <c r="H24" s="44"/>
+      <c r="I24" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="J24" s="17"/>
-      <c r="K24" s="16" t="s">
+      <c r="J24" s="16"/>
+      <c r="K24" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="L24" s="17"/>
-      <c r="M24" s="16">
+      <c r="L24" s="16"/>
+      <c r="M24" s="17">
         <v>2</v>
       </c>
-      <c r="N24" s="17"/>
-      <c r="O24" s="16" t="s">
+      <c r="N24" s="16"/>
+      <c r="O24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="17"/>
-    </row>
-    <row r="25" spans="1:18" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="P24" s="16"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="16"/>
+    </row>
+    <row r="25" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="7" t="s">
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="60" t="s">
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25" s="44"/>
+      <c r="I25" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25" s="62"/>
+      <c r="K25" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="L25" s="14"/>
+      <c r="M25" s="23">
+        <v>1</v>
+      </c>
+      <c r="N25" s="14"/>
+      <c r="O25" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="23">
+        <v>1</v>
+      </c>
+      <c r="R25" s="14"/>
+    </row>
+    <row r="26" spans="1:18" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="59"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H25" s="60"/>
-      <c r="I25" s="12" t="s">
+      <c r="H26" s="3"/>
+      <c r="I26" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="J25" s="13"/>
-      <c r="K25" s="12" t="s">
+      <c r="J26" s="2"/>
+      <c r="K26" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="L25" s="13"/>
-      <c r="M25" s="12">
+      <c r="L26" s="2"/>
+      <c r="M26" s="19">
         <v>2</v>
       </c>
-      <c r="N25" s="13"/>
-      <c r="O25" s="12" t="s">
+      <c r="N26" s="2"/>
+      <c r="O26" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="12">
+      <c r="P26" s="2"/>
+      <c r="Q26" s="19">
         <v>1</v>
       </c>
-      <c r="R25" s="13"/>
-    </row>
-    <row r="26" spans="1:18" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="58"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="60" t="s">
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:18" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="59"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H26" s="60"/>
-      <c r="I26" s="59" t="s">
+      <c r="H27" s="3"/>
+      <c r="I27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J26" s="11"/>
-      <c r="K26" s="20" t="s">
+      <c r="J27" s="2"/>
+      <c r="K27" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="L26" s="11"/>
-      <c r="M26" s="20">
+      <c r="L27" s="2"/>
+      <c r="M27" s="19">
         <v>1</v>
       </c>
-      <c r="N26" s="11"/>
-      <c r="O26" s="20" t="s">
+      <c r="N27" s="2"/>
+      <c r="O27" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="20">
+      <c r="P27" s="2"/>
+      <c r="Q27" s="19">
         <v>1</v>
       </c>
-      <c r="R26" s="11"/>
-    </row>
-    <row r="27" spans="1:18" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="60" t="s">
+      <c r="R27" s="2"/>
+    </row>
+    <row r="28" spans="1:18" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H27" s="60"/>
-      <c r="I27" s="19" t="s">
+      <c r="H28" s="3"/>
+      <c r="I28" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="J27" s="17"/>
-      <c r="K27" s="16" t="s">
+      <c r="J28" s="16"/>
+      <c r="K28" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L27" s="17"/>
-      <c r="M27" s="43">
+      <c r="L28" s="16"/>
+      <c r="M28" s="18">
         <v>1</v>
       </c>
-      <c r="N27" s="17"/>
-      <c r="O27" s="43" t="s">
+      <c r="N28" s="16"/>
+      <c r="O28" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="16">
+      <c r="P28" s="16"/>
+      <c r="Q28" s="17">
         <v>1</v>
       </c>
-      <c r="R27" s="17"/>
+      <c r="R28" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="124">
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A25:C27"/>
-    <mergeCell ref="D25:F27"/>
+  <mergeCells count="130">
+    <mergeCell ref="A25:C28"/>
+    <mergeCell ref="D25:F28"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="M25:N25"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="A13:C18"/>
-    <mergeCell ref="D13:F18"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="A2:B7"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="H4:O4"/>
-    <mergeCell ref="H5:O6"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A19:C21"/>
     <mergeCell ref="D19:F21"/>
     <mergeCell ref="Q23:R23"/>
@@ -1868,6 +1820,104 @@
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="K17:L17"/>
+    <mergeCell ref="A2:B7"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="H4:O4"/>
+    <mergeCell ref="H5:O6"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="A13:C18"/>
+    <mergeCell ref="D13:F18"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O26:P26"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1879,166 +1929,148 @@
   <dimension ref="D5:K12"/>
   <sheetViews>
     <sheetView zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="5" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44" t="s">
+      <c r="E5" s="54"/>
+      <c r="F5" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44" t="s">
+      <c r="G5" s="54"/>
+      <c r="H5" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44" t="s">
+      <c r="I5" s="54"/>
+      <c r="J5" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="44"/>
+      <c r="K5" s="54"/>
     </row>
     <row r="6" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="45">
+      <c r="E6" s="56"/>
+      <c r="F6" s="55">
         <v>13</v>
       </c>
-      <c r="G6" s="46"/>
-      <c r="H6" s="45">
+      <c r="G6" s="56"/>
+      <c r="H6" s="55">
         <v>12</v>
       </c>
-      <c r="I6" s="46"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="50"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="58"/>
     </row>
     <row r="7" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="48"/>
-      <c r="F7" s="47">
+      <c r="E7" s="47"/>
+      <c r="F7" s="46">
         <v>8</v>
       </c>
-      <c r="G7" s="48"/>
-      <c r="H7" s="47">
+      <c r="G7" s="47"/>
+      <c r="H7" s="46">
         <v>9</v>
       </c>
-      <c r="I7" s="48"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="51"/>
     </row>
     <row r="8" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="48"/>
-      <c r="F8" s="47">
+      <c r="E8" s="47"/>
+      <c r="F8" s="46">
         <v>5</v>
       </c>
-      <c r="G8" s="48"/>
-      <c r="H8" s="47">
-        <v>4</v>
-      </c>
-      <c r="I8" s="48"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="52"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="46">
+        <v>5</v>
+      </c>
+      <c r="I8" s="47"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="51"/>
     </row>
     <row r="9" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="48"/>
-      <c r="F9" s="47">
+      <c r="E9" s="47"/>
+      <c r="F9" s="46">
+        <v>8</v>
+      </c>
+      <c r="G9" s="47"/>
+      <c r="H9" s="46">
+        <v>7</v>
+      </c>
+      <c r="I9" s="47"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="51"/>
+    </row>
+    <row r="10" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="47"/>
+      <c r="F10" s="46">
         <v>6</v>
       </c>
-      <c r="G9" s="48"/>
-      <c r="H9" s="47">
+      <c r="G10" s="47"/>
+      <c r="H10" s="46">
         <v>6</v>
       </c>
-      <c r="I9" s="48"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="52"/>
-    </row>
-    <row r="10" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="48"/>
-      <c r="F10" s="47">
+      <c r="I10" s="47"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="51"/>
+    </row>
+    <row r="11" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="48">
+        <v>7</v>
+      </c>
+      <c r="G11" s="49"/>
+      <c r="H11" s="48">
         <v>6</v>
       </c>
-      <c r="G10" s="48"/>
-      <c r="H10" s="47">
-        <v>6</v>
-      </c>
-      <c r="I10" s="48"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
-    </row>
-    <row r="11" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="57"/>
-      <c r="F11" s="56">
-        <v>7</v>
-      </c>
-      <c r="G11" s="57"/>
-      <c r="H11" s="56">
-        <v>6</v>
-      </c>
-      <c r="I11" s="57"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="55"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="53"/>
     </row>
     <row r="12" spans="4:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53">
+      <c r="E12" s="45"/>
+      <c r="F12" s="45">
         <f>SUM(F6,F7,F8,F9,F10,F11)</f>
+        <v>47</v>
+      </c>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45">
+        <f>SUM(H6:I11)</f>
         <v>45</v>
       </c>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53">
-        <f>SUM(H6:I11)</f>
-        <v>43</v>
-      </c>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53">
+      <c r="I12" s="45"/>
+      <c r="J12" s="45">
         <f>SUM(J6:K11)</f>
         <v>0</v>
       </c>
-      <c r="K12" s="53"/>
+      <c r="K12" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J11:K11"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
@@ -2053,6 +2085,24 @@
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update release#5 planning sheet
</commit_message>
<xml_diff>
--- a/PMP/Release Planning/Release#5_planning.xlsx
+++ b/PMP/Release Planning/Release#5_planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Engineer\OneDrive - MUST University\Desktop\Release#5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Engineer\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1FDBDD-2414-473B-9904-4EAE761DC007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2949362D-020B-49FE-8B38-4549AF0C4A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{09E57C9E-5FED-45FA-83CB-16D2930F95A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{09E57C9E-5FED-45FA-83CB-16D2930F95A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Release Planning" sheetId="1" r:id="rId1"/>
@@ -554,67 +554,106 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -622,9 +661,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -652,49 +688,46 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -702,45 +735,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1080,7 +1074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{756EBB98-C920-47B4-A4C0-6F8760196D70}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
@@ -1095,749 +1089,739 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="H1" s="35" t="s">
+      <c r="D1" s="31"/>
+      <c r="H1" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="37"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="28"/>
     </row>
     <row r="2" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="42" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="H2" s="38" t="s">
+      <c r="D2" s="33"/>
+      <c r="H2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38" t="s">
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
     </row>
     <row r="3" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="42" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="H3" s="39">
+      <c r="D3" s="33"/>
+      <c r="H3" s="30">
         <v>45935</v>
       </c>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="39" t="s">
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
     </row>
     <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="42" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="H4" s="38" t="s">
+      <c r="D4" s="33"/>
+      <c r="H4" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
     </row>
     <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="42" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="H5" s="40" t="s">
+      <c r="D5" s="33"/>
+      <c r="H5" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
     </row>
     <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="42" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
+      <c r="D6" s="33"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
     </row>
     <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="42" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="42"/>
-      <c r="H7" s="40" t="s">
+      <c r="D7" s="33"/>
+      <c r="H7" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40" t="s">
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
     </row>
     <row r="12" spans="1:18" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21" t="s">
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21" t="s">
+      <c r="H12" s="34"/>
+      <c r="I12" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21" t="s">
+      <c r="J12" s="34"/>
+      <c r="K12" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="21"/>
-      <c r="M12" s="22" t="s">
+      <c r="L12" s="34"/>
+      <c r="M12" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="N12" s="22"/>
-      <c r="O12" s="21" t="s">
+      <c r="N12" s="35"/>
+      <c r="O12" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21" t="s">
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="R12" s="21"/>
+      <c r="R12" s="34"/>
     </row>
     <row r="13" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="24" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="13" t="s">
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="13" t="s">
+      <c r="H13" s="15"/>
+      <c r="I13" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="13" t="s">
+      <c r="J13" s="15"/>
+      <c r="K13" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="13">
+      <c r="L13" s="15"/>
+      <c r="M13" s="18">
         <v>2</v>
       </c>
-      <c r="N13" s="14"/>
-      <c r="O13" s="23" t="s">
+      <c r="N13" s="15"/>
+      <c r="O13" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="13">
+      <c r="P13" s="15"/>
+      <c r="Q13" s="18">
         <v>1</v>
       </c>
-      <c r="R13" s="14"/>
+      <c r="R13" s="15"/>
     </row>
     <row r="14" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="13" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="1" t="s">
+      <c r="H14" s="15"/>
+      <c r="I14" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="1" t="s">
+      <c r="J14" s="17"/>
+      <c r="K14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="19">
+      <c r="L14" s="17"/>
+      <c r="M14" s="23">
         <v>4</v>
       </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="19" t="s">
+      <c r="N14" s="17"/>
+      <c r="O14" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="1">
+      <c r="P14" s="17"/>
+      <c r="Q14" s="16">
         <v>1</v>
       </c>
-      <c r="R14" s="2"/>
+      <c r="R14" s="17"/>
     </row>
     <row r="15" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="13" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="1" t="s">
+      <c r="H15" s="15"/>
+      <c r="I15" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="1" t="s">
+      <c r="J15" s="17"/>
+      <c r="K15" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="19">
+      <c r="L15" s="17"/>
+      <c r="M15" s="23">
         <v>4</v>
       </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="19" t="s">
+      <c r="N15" s="17"/>
+      <c r="O15" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="1">
+      <c r="P15" s="17"/>
+      <c r="Q15" s="16">
         <v>1</v>
       </c>
-      <c r="R15" s="2"/>
+      <c r="R15" s="17"/>
     </row>
     <row r="16" spans="1:18" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="13" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="20" t="s">
+      <c r="H16" s="15"/>
+      <c r="I16" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="1" t="s">
+      <c r="J16" s="17"/>
+      <c r="K16" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L16" s="2"/>
-      <c r="M16" s="19">
+      <c r="L16" s="17"/>
+      <c r="M16" s="23">
         <v>2</v>
       </c>
-      <c r="N16" s="2"/>
-      <c r="O16" s="19" t="s">
+      <c r="N16" s="17"/>
+      <c r="O16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="1">
+      <c r="P16" s="17"/>
+      <c r="Q16" s="16">
         <v>1</v>
       </c>
-      <c r="R16" s="2"/>
+      <c r="R16" s="17"/>
     </row>
     <row r="17" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="13" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="1" t="s">
+      <c r="H17" s="15"/>
+      <c r="I17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="1" t="s">
+      <c r="J17" s="17"/>
+      <c r="K17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="19">
+      <c r="L17" s="17"/>
+      <c r="M17" s="23">
         <v>2</v>
       </c>
-      <c r="N17" s="2"/>
-      <c r="O17" s="19" t="s">
+      <c r="N17" s="17"/>
+      <c r="O17" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="1">
+      <c r="P17" s="17"/>
+      <c r="Q17" s="16">
         <v>1</v>
       </c>
-      <c r="R17" s="2"/>
+      <c r="R17" s="17"/>
     </row>
     <row r="18" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="13" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="20" t="s">
+      <c r="H18" s="15"/>
+      <c r="I18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="1" t="s">
+      <c r="J18" s="17"/>
+      <c r="K18" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="19">
+      <c r="L18" s="17"/>
+      <c r="M18" s="23">
         <v>2</v>
       </c>
-      <c r="N18" s="2"/>
-      <c r="O18" s="19" t="s">
+      <c r="N18" s="17"/>
+      <c r="O18" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="1">
+      <c r="P18" s="17"/>
+      <c r="Q18" s="16">
         <v>1</v>
       </c>
-      <c r="R18" s="2"/>
+      <c r="R18" s="17"/>
     </row>
     <row r="19" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="10" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="13" t="s">
+      <c r="E19" s="1"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="13" t="s">
+      <c r="H19" s="15"/>
+      <c r="I19" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="J19" s="14"/>
-      <c r="K19" s="13" t="s">
+      <c r="J19" s="15"/>
+      <c r="K19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="14"/>
-      <c r="M19" s="13">
+      <c r="L19" s="15"/>
+      <c r="M19" s="18">
         <v>2</v>
       </c>
-      <c r="N19" s="14"/>
-      <c r="O19" s="13" t="s">
+      <c r="N19" s="15"/>
+      <c r="O19" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="13">
+      <c r="P19" s="15"/>
+      <c r="Q19" s="18">
         <v>1</v>
       </c>
-      <c r="R19" s="14"/>
+      <c r="R19" s="15"/>
     </row>
     <row r="20" spans="1:18" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="13" t="s">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="20" t="s">
+      <c r="H20" s="15"/>
+      <c r="I20" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="1" t="s">
+      <c r="J20" s="17"/>
+      <c r="K20" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="2"/>
-      <c r="M20" s="19">
+      <c r="L20" s="17"/>
+      <c r="M20" s="23">
         <v>2</v>
       </c>
-      <c r="N20" s="2"/>
-      <c r="O20" s="19" t="s">
+      <c r="N20" s="17"/>
+      <c r="O20" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="1">
+      <c r="P20" s="17"/>
+      <c r="Q20" s="16">
         <v>1</v>
       </c>
-      <c r="R20" s="2"/>
+      <c r="R20" s="17"/>
     </row>
     <row r="21" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="13" t="s">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="14"/>
-      <c r="I21" s="17" t="s">
+      <c r="H21" s="15"/>
+      <c r="I21" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="J21" s="16"/>
-      <c r="K21" s="17" t="s">
+      <c r="J21" s="20"/>
+      <c r="K21" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="16"/>
-      <c r="M21" s="18">
+      <c r="L21" s="20"/>
+      <c r="M21" s="45">
         <v>2</v>
       </c>
-      <c r="N21" s="16"/>
-      <c r="O21" s="18" t="s">
+      <c r="N21" s="20"/>
+      <c r="O21" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="17">
+      <c r="P21" s="20"/>
+      <c r="Q21" s="19">
         <v>1</v>
       </c>
-      <c r="R21" s="16"/>
+      <c r="R21" s="20"/>
     </row>
     <row r="22" spans="1:18" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="10" t="s">
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="13" t="s">
+      <c r="E22" s="1"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="1" t="s">
+      <c r="H22" s="15"/>
+      <c r="I22" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="1" t="s">
+      <c r="J22" s="17"/>
+      <c r="K22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="1">
+      <c r="L22" s="17"/>
+      <c r="M22" s="16">
         <v>2</v>
       </c>
-      <c r="N22" s="2"/>
-      <c r="O22" s="1" t="s">
+      <c r="N22" s="17"/>
+      <c r="O22" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="2"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="17"/>
     </row>
     <row r="23" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="13" t="s">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="20" t="s">
+      <c r="H23" s="15"/>
+      <c r="I23" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="1" t="s">
+      <c r="J23" s="17"/>
+      <c r="K23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L23" s="2"/>
-      <c r="M23" s="1">
+      <c r="L23" s="17"/>
+      <c r="M23" s="16">
         <v>2</v>
       </c>
-      <c r="N23" s="2"/>
-      <c r="O23" s="1" t="s">
+      <c r="N23" s="17"/>
+      <c r="O23" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="2"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="17"/>
     </row>
     <row r="24" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="43" t="s">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="H24" s="44"/>
-      <c r="I24" s="15" t="s">
+      <c r="H24" s="11"/>
+      <c r="I24" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="J24" s="16"/>
-      <c r="K24" s="17" t="s">
+      <c r="J24" s="20"/>
+      <c r="K24" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="L24" s="16"/>
-      <c r="M24" s="17">
+      <c r="L24" s="20"/>
+      <c r="M24" s="19">
         <v>2</v>
       </c>
-      <c r="N24" s="16"/>
-      <c r="O24" s="17" t="s">
+      <c r="N24" s="20"/>
+      <c r="O24" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="16"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="20"/>
     </row>
     <row r="25" spans="1:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="10" t="s">
+      <c r="B25" s="1"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="43" t="s">
+      <c r="E25" s="1"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="44"/>
-      <c r="I25" s="61" t="s">
+      <c r="H25" s="11"/>
+      <c r="I25" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="J25" s="62"/>
-      <c r="K25" s="23" t="s">
+      <c r="J25" s="13"/>
+      <c r="K25" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="L25" s="14"/>
-      <c r="M25" s="23">
+      <c r="L25" s="15"/>
+      <c r="M25" s="14">
         <v>1</v>
       </c>
-      <c r="N25" s="14"/>
-      <c r="O25" s="23" t="s">
+      <c r="N25" s="15"/>
+      <c r="O25" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="23">
+      <c r="P25" s="15"/>
+      <c r="Q25" s="14">
         <v>1</v>
       </c>
-      <c r="R25" s="14"/>
+      <c r="R25" s="15"/>
     </row>
     <row r="26" spans="1:18" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="59"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="3" t="s">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="H26" s="3"/>
-      <c r="I26" s="19" t="s">
+      <c r="H26" s="46"/>
+      <c r="I26" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="J26" s="2"/>
-      <c r="K26" s="19" t="s">
+      <c r="J26" s="17"/>
+      <c r="K26" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="L26" s="2"/>
-      <c r="M26" s="19">
+      <c r="L26" s="17"/>
+      <c r="M26" s="23">
         <v>2</v>
       </c>
-      <c r="N26" s="2"/>
-      <c r="O26" s="60" t="s">
+      <c r="N26" s="17"/>
+      <c r="O26" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="19">
+      <c r="P26" s="17"/>
+      <c r="Q26" s="23">
         <v>1</v>
       </c>
-      <c r="R26" s="2"/>
+      <c r="R26" s="17"/>
     </row>
     <row r="27" spans="1:18" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="59"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="3" t="s">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="1" t="s">
+      <c r="H27" s="46"/>
+      <c r="I27" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="J27" s="2"/>
-      <c r="K27" s="19" t="s">
+      <c r="J27" s="17"/>
+      <c r="K27" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="L27" s="2"/>
-      <c r="M27" s="19">
+      <c r="L27" s="17"/>
+      <c r="M27" s="23">
         <v>1</v>
       </c>
-      <c r="N27" s="2"/>
-      <c r="O27" s="19" t="s">
+      <c r="N27" s="17"/>
+      <c r="O27" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="19">
+      <c r="P27" s="17"/>
+      <c r="Q27" s="23">
         <v>1</v>
       </c>
-      <c r="R27" s="2"/>
+      <c r="R27" s="17"/>
     </row>
     <row r="28" spans="1:18" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="3" t="s">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="15" t="s">
+      <c r="H28" s="46"/>
+      <c r="I28" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="J28" s="16"/>
-      <c r="K28" s="17" t="s">
+      <c r="J28" s="20"/>
+      <c r="K28" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="L28" s="16"/>
-      <c r="M28" s="18">
+      <c r="L28" s="20"/>
+      <c r="M28" s="45">
         <v>1</v>
       </c>
-      <c r="N28" s="16"/>
-      <c r="O28" s="18" t="s">
+      <c r="N28" s="20"/>
+      <c r="O28" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="17">
+      <c r="P28" s="20"/>
+      <c r="Q28" s="19">
         <v>1</v>
       </c>
-      <c r="R28" s="16"/>
+      <c r="R28" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="130">
-    <mergeCell ref="A25:C28"/>
-    <mergeCell ref="D25:F28"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="A19:C21"/>
-    <mergeCell ref="D19:F21"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="A22:C24"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="D22:F24"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="A2:B7"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="H4:O4"/>
-    <mergeCell ref="H5:O6"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O12:P12"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G12:H12"/>
@@ -1862,44 +1846,63 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
+    <mergeCell ref="A2:B7"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="H4:O4"/>
+    <mergeCell ref="H5:O6"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="A22:C24"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="D22:F24"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="I19:J19"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q19:R19"/>
     <mergeCell ref="O19:P19"/>
     <mergeCell ref="K19:L19"/>
+    <mergeCell ref="A25:C28"/>
+    <mergeCell ref="D25:F28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="A19:C21"/>
+    <mergeCell ref="D19:F21"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="Q19:R19"/>
     <mergeCell ref="M19:N19"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="O20:P20"/>
     <mergeCell ref="Q26:R26"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="I28:J28"/>
@@ -1909,15 +1912,6 @@
     <mergeCell ref="Q28:R28"/>
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="O27:P27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O26:P26"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1928,149 +1922,179 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC208F04-60BB-4D9F-8E98-D4B507CD0159}">
   <dimension ref="D5:K12"/>
   <sheetViews>
-    <sheetView zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="5" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54" t="s">
+      <c r="E5" s="47"/>
+      <c r="F5" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54" t="s">
+      <c r="G5" s="47"/>
+      <c r="H5" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54" t="s">
+      <c r="I5" s="47"/>
+      <c r="J5" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="54"/>
+      <c r="K5" s="47"/>
     </row>
     <row r="6" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="56"/>
-      <c r="F6" s="55">
+      <c r="E6" s="49"/>
+      <c r="F6" s="48">
         <v>13</v>
       </c>
-      <c r="G6" s="56"/>
-      <c r="H6" s="55">
+      <c r="G6" s="49"/>
+      <c r="H6" s="48">
         <v>12</v>
       </c>
-      <c r="I6" s="56"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="58"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="52">
+        <v>11.5</v>
+      </c>
+      <c r="K6" s="53"/>
     </row>
     <row r="7" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="46">
+      <c r="E7" s="51"/>
+      <c r="F7" s="50">
         <v>8</v>
       </c>
-      <c r="G7" s="47"/>
-      <c r="H7" s="46">
+      <c r="G7" s="51"/>
+      <c r="H7" s="50">
         <v>9</v>
       </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="54">
+        <v>8</v>
+      </c>
+      <c r="K7" s="55"/>
     </row>
     <row r="8" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="47"/>
-      <c r="F8" s="46">
+      <c r="E8" s="51"/>
+      <c r="F8" s="50">
         <v>5</v>
       </c>
-      <c r="G8" s="47"/>
-      <c r="H8" s="46">
+      <c r="G8" s="51"/>
+      <c r="H8" s="50">
         <v>5</v>
       </c>
-      <c r="I8" s="47"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="54">
+        <v>4</v>
+      </c>
+      <c r="K8" s="55"/>
     </row>
     <row r="9" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="47"/>
-      <c r="F9" s="46">
+      <c r="E9" s="51"/>
+      <c r="F9" s="50">
         <v>8</v>
       </c>
-      <c r="G9" s="47"/>
-      <c r="H9" s="46">
+      <c r="G9" s="51"/>
+      <c r="H9" s="50">
         <v>7</v>
       </c>
-      <c r="I9" s="47"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="54">
+        <v>7</v>
+      </c>
+      <c r="K9" s="55"/>
     </row>
     <row r="10" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="46">
+      <c r="E10" s="51"/>
+      <c r="F10" s="50">
         <v>6</v>
       </c>
-      <c r="G10" s="47"/>
-      <c r="H10" s="46">
+      <c r="G10" s="51"/>
+      <c r="H10" s="50">
         <v>6</v>
       </c>
-      <c r="I10" s="47"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="54">
+        <v>5.5</v>
+      </c>
+      <c r="K10" s="55"/>
     </row>
     <row r="11" spans="4:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="49"/>
-      <c r="F11" s="48">
+      <c r="E11" s="60"/>
+      <c r="F11" s="59">
         <v>7</v>
       </c>
-      <c r="G11" s="49"/>
-      <c r="H11" s="48">
+      <c r="G11" s="60"/>
+      <c r="H11" s="59">
         <v>6</v>
       </c>
-      <c r="I11" s="49"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="53"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="57">
+        <v>6</v>
+      </c>
+      <c r="K11" s="58"/>
     </row>
     <row r="12" spans="4:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45">
+      <c r="E12" s="56"/>
+      <c r="F12" s="56">
         <f>SUM(F6,F7,F8,F9,F10,F11)</f>
         <v>47</v>
       </c>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45">
+      <c r="G12" s="56"/>
+      <c r="H12" s="56">
         <f>SUM(H6:I11)</f>
         <v>45</v>
       </c>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45">
+      <c r="I12" s="56"/>
+      <c r="J12" s="56">
         <f>SUM(J6:K11)</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="45"/>
+        <v>42</v>
+      </c>
+      <c r="K12" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J11:K11"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
@@ -2085,24 +2109,6 @@
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>